<commit_message>
Add component connections related functions Refactor the relation functions
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming Workspace\Knowledge Graph\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming Workspace\Knowledge Graphs\My_MscProject\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EC2E374-C0D1-4986-8928-C274D990227F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA23F3B4-9E0B-473D-AB8C-9E763DB841E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="752" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="752" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Family" sheetId="7" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3506" uniqueCount="885">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3506" uniqueCount="886">
   <si>
     <t>Engine</t>
   </si>
@@ -7691,9 +7691,6 @@
   </si>
   <si>
     <t>Slip Fit</t>
-  </si>
-  <si>
-    <t>[(3, 'C0010011')]</t>
   </si>
   <si>
     <t>[(1, 'C0010005')]</t>
@@ -7813,6 +7810,14 @@
   </si>
   <si>
     <t>Inventory</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>C0010009</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>[(3, 'C0010011')]</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -9174,8 +9179,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{305198D0-9831-4C68-8821-C572C13460ED}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -9186,10 +9191,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
@@ -9307,8 +9312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{767E015E-E14A-411A-85C5-82BE42749A86}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -9330,7 +9335,7 @@
         <v>73</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>69</v>
@@ -9354,7 +9359,7 @@
         <v>126</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="K1" s="7" t="s">
         <v>42</v>
@@ -9380,7 +9385,7 @@
         <v>95</v>
       </c>
       <c r="G2" s="155" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="H2" s="151" t="s">
         <v>34</v>
@@ -9392,7 +9397,7 @@
         <v>490</v>
       </c>
       <c r="K2" s="156" t="s">
-        <v>853</v>
+        <v>885</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
@@ -9415,7 +9420,7 @@
         <v>95</v>
       </c>
       <c r="G3" s="155" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="H3" s="151" t="s">
         <v>34</v>
@@ -9427,7 +9432,7 @@
         <v>552</v>
       </c>
       <c r="K3" s="156" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
@@ -9450,7 +9455,7 @@
         <v>95</v>
       </c>
       <c r="G4" s="155" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="H4" s="151" t="s">
         <v>119</v>
@@ -9462,7 +9467,7 @@
         <v>468</v>
       </c>
       <c r="K4" s="156" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
@@ -9485,7 +9490,7 @@
         <v>95</v>
       </c>
       <c r="G5" s="155" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="H5" s="151" t="s">
         <v>119</v>
@@ -9497,7 +9502,7 @@
         <v>571</v>
       </c>
       <c r="K5" s="156" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
@@ -9520,7 +9525,7 @@
         <v>95</v>
       </c>
       <c r="G6" s="155" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="H6" s="151" t="s">
         <v>127</v>
@@ -9532,7 +9537,7 @@
         <v>341</v>
       </c>
       <c r="K6" s="156" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
@@ -9555,7 +9560,7 @@
         <v>95</v>
       </c>
       <c r="G7" s="155" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="H7" s="151" t="s">
         <v>127</v>
@@ -9567,7 +9572,7 @@
         <v>424</v>
       </c>
       <c r="K7" s="156" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
@@ -9590,7 +9595,7 @@
         <v>96</v>
       </c>
       <c r="G8" s="155" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="H8" s="151" t="s">
         <v>128</v>
@@ -9602,7 +9607,7 @@
         <v>605</v>
       </c>
       <c r="K8" s="156" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
@@ -9625,7 +9630,7 @@
         <v>96</v>
       </c>
       <c r="G9" s="155" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="H9" s="151" t="s">
         <v>128</v>
@@ -9637,12 +9642,12 @@
         <v>411</v>
       </c>
       <c r="K9" s="156" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A10" s="151" t="s">
-        <v>83</v>
+        <v>884</v>
       </c>
       <c r="B10" s="152" t="s">
         <v>53</v>
@@ -9672,7 +9677,7 @@
         <v>745</v>
       </c>
       <c r="K10" s="156" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
@@ -9707,7 +9712,7 @@
         <v>915</v>
       </c>
       <c r="K11" s="156" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
@@ -9730,7 +9735,7 @@
         <v>96</v>
       </c>
       <c r="G12" s="155" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="H12" s="151" t="s">
         <v>130</v>
@@ -9742,7 +9747,7 @@
         <v>541</v>
       </c>
       <c r="K12" s="156" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
@@ -9765,7 +9770,7 @@
         <v>96</v>
       </c>
       <c r="G13" s="155" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="H13" s="151" t="s">
         <v>130</v>
@@ -9777,7 +9782,7 @@
         <v>388</v>
       </c>
       <c r="K13" s="156" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
@@ -9800,7 +9805,7 @@
         <v>97</v>
       </c>
       <c r="G14" s="155" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="H14" s="151" t="s">
         <v>131</v>
@@ -9812,7 +9817,7 @@
         <v>987</v>
       </c>
       <c r="K14" s="156" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
@@ -9835,7 +9840,7 @@
         <v>97</v>
       </c>
       <c r="G15" s="155" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="H15" s="151" t="s">
         <v>131</v>
@@ -9847,7 +9852,7 @@
         <v>732</v>
       </c>
       <c r="K15" s="156" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
@@ -9870,7 +9875,7 @@
         <v>97</v>
       </c>
       <c r="G16" s="155" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="H16" s="151" t="s">
         <v>131</v>
@@ -9882,7 +9887,7 @@
         <v>642</v>
       </c>
       <c r="K16" s="156" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
@@ -9905,7 +9910,7 @@
         <v>97</v>
       </c>
       <c r="G17" s="155" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="H17" s="151" t="s">
         <v>132</v>
@@ -9917,7 +9922,7 @@
         <v>711</v>
       </c>
       <c r="K17" s="156" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
@@ -9940,7 +9945,7 @@
         <v>97</v>
       </c>
       <c r="G18" s="155" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="H18" s="151" t="s">
         <v>132</v>
@@ -9952,7 +9957,7 @@
         <v>548</v>
       </c>
       <c r="K18" s="156" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
@@ -9975,7 +9980,7 @@
         <v>97</v>
       </c>
       <c r="G19" s="155" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="H19" s="151" t="s">
         <v>132</v>
@@ -9987,7 +9992,7 @@
         <v>841</v>
       </c>
       <c r="K19" s="156" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
@@ -10010,7 +10015,7 @@
         <v>97</v>
       </c>
       <c r="G20" s="155" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="H20" s="151" t="s">
         <v>132</v>
@@ -10022,7 +10027,7 @@
         <v>547</v>
       </c>
       <c r="K20" s="156" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
     </row>
   </sheetData>
@@ -10897,7 +10902,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A14"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -10914,13 +10919,13 @@
         <v>32</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="C1" s="158" t="s">
         <v>33</v>
       </c>
       <c r="D1" s="159" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="E1" s="157"/>
       <c r="F1" s="157"/>
@@ -10934,7 +10939,7 @@
         <v>13</v>
       </c>
       <c r="C2" s="161" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="D2" s="160" t="s">
         <v>39</v>
@@ -10948,7 +10953,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="161" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="D3" s="160" t="s">
         <v>39</v>
@@ -10962,7 +10967,7 @@
         <v>15</v>
       </c>
       <c r="C4" s="161" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="D4" s="160" t="s">
         <v>39</v>
@@ -10976,7 +10981,7 @@
         <v>16</v>
       </c>
       <c r="C5" s="161" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="D5" s="160" t="s">
         <v>39</v>
@@ -10990,7 +10995,7 @@
         <v>17</v>
       </c>
       <c r="C6" s="161" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="D6" s="160" t="s">
         <v>39</v>
@@ -11004,7 +11009,7 @@
         <v>18</v>
       </c>
       <c r="C7" s="161" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="D7" s="160" t="s">
         <v>39</v>
@@ -11018,7 +11023,7 @@
         <v>19</v>
       </c>
       <c r="C8" s="161" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="D8" s="160" t="s">
         <v>40</v>
@@ -11032,7 +11037,7 @@
         <v>20</v>
       </c>
       <c r="C9" s="161" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="D9" s="160" t="s">
         <v>40</v>
@@ -11046,7 +11051,7 @@
         <v>21</v>
       </c>
       <c r="C10" s="161" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="D10" s="160" t="s">
         <v>40</v>
@@ -11060,7 +11065,7 @@
         <v>22</v>
       </c>
       <c r="C11" s="161" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="D11" s="160" t="s">
         <v>40</v>
@@ -11074,7 +11079,7 @@
         <v>23</v>
       </c>
       <c r="C12" s="161" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="D12" s="160" t="s">
         <v>40</v>
@@ -11088,7 +11093,7 @@
         <v>24</v>
       </c>
       <c r="C13" s="161" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="D13" s="160" t="s">
         <v>40</v>
@@ -11102,7 +11107,7 @@
         <v>25</v>
       </c>
       <c r="C14" s="161" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="D14" s="160" t="s">
         <v>40</v>
@@ -11116,7 +11121,7 @@
         <v>26</v>
       </c>
       <c r="C15" s="161" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="D15" s="160" t="s">
         <v>41</v>
@@ -11130,7 +11135,7 @@
         <v>27</v>
       </c>
       <c r="C16" s="161" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="D16" s="160" t="s">
         <v>41</v>
@@ -11144,7 +11149,7 @@
         <v>28</v>
       </c>
       <c r="C17" s="161" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="D17" s="160" t="s">
         <v>41</v>
@@ -11158,7 +11163,7 @@
         <v>29</v>
       </c>
       <c r="C18" s="161" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="D18" s="160" t="s">
         <v>41</v>
@@ -11172,7 +11177,7 @@
         <v>30</v>
       </c>
       <c r="C19" s="161" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="D19" s="160" t="s">
         <v>41</v>
@@ -11186,7 +11191,7 @@
         <v>31</v>
       </c>
       <c r="C20" s="161" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="D20" s="160" t="s">
         <v>41</v>
@@ -27460,7 +27465,7 @@
         <v>118</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add dataset for embeddings
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming Workspace\Knowledge Graphs\My_MscProject\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA23F3B4-9E0B-473D-AB8C-9E763DB841E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB6A1B09-07C5-4762-8BA9-C2DA5AC26739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="752" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="752" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Family" sheetId="7" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3506" uniqueCount="886">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3506" uniqueCount="888">
   <si>
     <t>Engine</t>
   </si>
@@ -7693,49 +7693,10 @@
     <t>Slip Fit</t>
   </si>
   <si>
-    <t>[(1, 'C0010005')]</t>
-  </si>
-  <si>
-    <t>[(1, 'C0010014')]</t>
-  </si>
-  <si>
     <t>[(6, 'C0010017'), (10, 'C0010017')]</t>
   </si>
   <si>
-    <t>[(1, 'C0010009'), (7, 'C0010009'), (8, 'C0010009')]</t>
-  </si>
-  <si>
-    <t>[(1, 'C0010009')]</t>
-  </si>
-  <si>
-    <t>[(7, 'C0010019')]</t>
-  </si>
-  <si>
-    <t>[(3, 'C0010018')]</t>
-  </si>
-  <si>
-    <t>[(7, 'C0010019'), (8, 'C0010019')]</t>
-  </si>
-  <si>
-    <t>[(1, 'C0010012')]</t>
-  </si>
-  <si>
-    <t>[(1, 'C0010007')]</t>
-  </si>
-  <si>
-    <t>[(6, 'C0010019')]</t>
-  </si>
-  <si>
     <t>[(1, 'C0010008')]</t>
-  </si>
-  <si>
-    <t>[(6, 'C0010018')]</t>
-  </si>
-  <si>
-    <t>[(3, 'C0010013')]</t>
-  </si>
-  <si>
-    <t>[(6, 'C0010016'), (10, 'C0010016')]</t>
   </si>
   <si>
     <t>[(3, 'C0010015')]</t>
@@ -7817,8 +7778,52 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>[(3, 'C0010011')]</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <t>[(1, 'C0010002'), (5, 'C0010005'), (10, 'C0010005'), (3, 'C0010011')]</t>
+  </si>
+  <si>
+    <t>[(1, 'C0010001'), (1, 'C0010005')]</t>
+  </si>
+  <si>
+    <t>[(5, 'C0010001'), (10, 'C0010001'), (1, 'C0010002'), (1, 'C0010004'), (1, 'C0010006'), (7, 'C0010010'), (8, 'C0010010'), (1, 'C0010014')]</t>
+  </si>
+  <si>
+    <t>[(3, 'C0010001'), (3, 'C0010015'), (6, 'C0010017'), (10, 'C0010017')]</t>
+  </si>
+  <si>
+    <t>[(1, 'C0010004'), (1, 'C0010009'), (7, 'C0010009'), (8, 'C0010009')]</t>
+  </si>
+  <si>
+    <t>[(1, 'C0010003'), (1, 'C0010005'), (1, 'C0010009')]</t>
+  </si>
+  <si>
+    <t>[(1, 'C0010003'), (7, 'C0010003'), (8, 'C0010003'), (1, 'C0010004'), (7, 'C0010019')]</t>
+  </si>
+  <si>
+    <t>[(1, 'C0010005'), (1, 'C0010008'), (3, 'C0010018')]</t>
+  </si>
+  <si>
+    <t>[(7, 'C0010005'), (8, 'C0010005'), (7, 'C0010012'), (8, 'C0010012'), (7, 'C0010019'), (8, 'C0010019')]</t>
+  </si>
+  <si>
+    <t>[(1, 'C0010005'), (1, 'C0010012')]</t>
+  </si>
+  <si>
+    <t>[(1, 'C0010006'), (1, 'C0010007')]</t>
+  </si>
+  <si>
+    <t>[(3, 'C0010006'), (6, 'C0010019')]</t>
+  </si>
+  <si>
+    <t>[(7, 'C0010009'), (7, 'C0010010'), (8, 'C0010010'), (6, 'C0010018')]</t>
+  </si>
+  <si>
+    <t>[(7, 'C0010010'), (8, 'C0010010'), (1, 'C0010014')]</t>
+  </si>
+  <si>
+    <t>[(3, 'C0010011'), (3, 'C0010013')]</t>
+  </si>
+  <si>
+    <t>[(6, 'C0010011'), (10, 'C0010011'), (6, 'C0010016'), (10, 'C0010016')]</t>
   </si>
 </sst>
 </file>
@@ -8813,9 +8818,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -8830,6 +8832,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -9191,10 +9196,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>872</v>
+        <v>859</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>871</v>
+        <v>858</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
@@ -9312,8 +9317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{767E015E-E14A-411A-85C5-82BE42749A86}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -9335,7 +9340,7 @@
         <v>73</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>870</v>
+        <v>857</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>69</v>
@@ -9359,7 +9364,7 @@
         <v>126</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>883</v>
+        <v>870</v>
       </c>
       <c r="K1" s="7" t="s">
         <v>42</v>
@@ -9385,7 +9390,7 @@
         <v>95</v>
       </c>
       <c r="G2" s="155" t="s">
-        <v>878</v>
+        <v>865</v>
       </c>
       <c r="H2" s="151" t="s">
         <v>34</v>
@@ -9396,8 +9401,8 @@
       <c r="J2" s="151">
         <v>490</v>
       </c>
-      <c r="K2" s="156" t="s">
-        <v>885</v>
+      <c r="K2" s="161" t="s">
+        <v>872</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
@@ -9420,7 +9425,7 @@
         <v>95</v>
       </c>
       <c r="G3" s="155" t="s">
-        <v>878</v>
+        <v>865</v>
       </c>
       <c r="H3" s="151" t="s">
         <v>34</v>
@@ -9431,8 +9436,8 @@
       <c r="J3" s="151">
         <v>552</v>
       </c>
-      <c r="K3" s="156" t="s">
-        <v>853</v>
+      <c r="K3" s="161" t="s">
+        <v>873</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
@@ -9455,7 +9460,7 @@
         <v>95</v>
       </c>
       <c r="G4" s="155" t="s">
-        <v>878</v>
+        <v>865</v>
       </c>
       <c r="H4" s="151" t="s">
         <v>119</v>
@@ -9466,8 +9471,8 @@
       <c r="J4" s="151">
         <v>468</v>
       </c>
-      <c r="K4" s="156" t="s">
-        <v>854</v>
+      <c r="K4" s="161" t="s">
+        <v>876</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
@@ -9490,7 +9495,7 @@
         <v>95</v>
       </c>
       <c r="G5" s="155" t="s">
-        <v>878</v>
+        <v>865</v>
       </c>
       <c r="H5" s="151" t="s">
         <v>119</v>
@@ -9501,8 +9506,8 @@
       <c r="J5" s="151">
         <v>571</v>
       </c>
-      <c r="K5" s="156" t="s">
-        <v>855</v>
+      <c r="K5" s="161" t="s">
+        <v>877</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
@@ -9525,7 +9530,7 @@
         <v>95</v>
       </c>
       <c r="G6" s="155" t="s">
-        <v>879</v>
+        <v>866</v>
       </c>
       <c r="H6" s="151" t="s">
         <v>127</v>
@@ -9536,8 +9541,8 @@
       <c r="J6" s="151">
         <v>341</v>
       </c>
-      <c r="K6" s="156" t="s">
-        <v>856</v>
+      <c r="K6" s="161" t="s">
+        <v>874</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
@@ -9560,7 +9565,7 @@
         <v>95</v>
       </c>
       <c r="G7" s="155" t="s">
-        <v>879</v>
+        <v>866</v>
       </c>
       <c r="H7" s="151" t="s">
         <v>127</v>
@@ -9571,8 +9576,8 @@
       <c r="J7" s="151">
         <v>424</v>
       </c>
-      <c r="K7" s="156" t="s">
-        <v>857</v>
+      <c r="K7" s="161" t="s">
+        <v>879</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
@@ -9595,7 +9600,7 @@
         <v>96</v>
       </c>
       <c r="G8" s="155" t="s">
-        <v>880</v>
+        <v>867</v>
       </c>
       <c r="H8" s="151" t="s">
         <v>128</v>
@@ -9606,8 +9611,8 @@
       <c r="J8" s="151">
         <v>605</v>
       </c>
-      <c r="K8" s="156" t="s">
-        <v>858</v>
+      <c r="K8" s="161" t="s">
+        <v>854</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
@@ -9630,7 +9635,7 @@
         <v>96</v>
       </c>
       <c r="G9" s="155" t="s">
-        <v>880</v>
+        <v>867</v>
       </c>
       <c r="H9" s="151" t="s">
         <v>128</v>
@@ -9641,13 +9646,13 @@
       <c r="J9" s="151">
         <v>411</v>
       </c>
-      <c r="K9" s="156" t="s">
-        <v>859</v>
+      <c r="K9" s="161" t="s">
+        <v>882</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A10" s="151" t="s">
-        <v>884</v>
+        <v>871</v>
       </c>
       <c r="B10" s="152" t="s">
         <v>53</v>
@@ -9676,8 +9681,8 @@
       <c r="J10" s="151">
         <v>745</v>
       </c>
-      <c r="K10" s="156" t="s">
-        <v>860</v>
+      <c r="K10" s="161" t="s">
+        <v>878</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
@@ -9711,8 +9716,8 @@
       <c r="J11" s="151">
         <v>915</v>
       </c>
-      <c r="K11" s="156" t="s">
-        <v>861</v>
+      <c r="K11" s="161" t="s">
+        <v>880</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
@@ -9735,7 +9740,7 @@
         <v>96</v>
       </c>
       <c r="G12" s="155" t="s">
-        <v>881</v>
+        <v>868</v>
       </c>
       <c r="H12" s="151" t="s">
         <v>130</v>
@@ -9746,8 +9751,8 @@
       <c r="J12" s="151">
         <v>541</v>
       </c>
-      <c r="K12" s="156" t="s">
-        <v>862</v>
+      <c r="K12" s="161" t="s">
+        <v>875</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
@@ -9770,7 +9775,7 @@
         <v>96</v>
       </c>
       <c r="G13" s="155" t="s">
-        <v>881</v>
+        <v>868</v>
       </c>
       <c r="H13" s="151" t="s">
         <v>130</v>
@@ -9781,8 +9786,8 @@
       <c r="J13" s="151">
         <v>388</v>
       </c>
-      <c r="K13" s="156" t="s">
-        <v>863</v>
+      <c r="K13" s="161" t="s">
+        <v>885</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
@@ -9805,7 +9810,7 @@
         <v>97</v>
       </c>
       <c r="G14" s="155" t="s">
-        <v>881</v>
+        <v>868</v>
       </c>
       <c r="H14" s="151" t="s">
         <v>131</v>
@@ -9816,8 +9821,8 @@
       <c r="J14" s="151">
         <v>987</v>
       </c>
-      <c r="K14" s="156" t="s">
-        <v>864</v>
+      <c r="K14" s="161" t="s">
+        <v>855</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
@@ -9840,7 +9845,7 @@
         <v>97</v>
       </c>
       <c r="G15" s="155" t="s">
-        <v>881</v>
+        <v>868</v>
       </c>
       <c r="H15" s="151" t="s">
         <v>131</v>
@@ -9851,8 +9856,8 @@
       <c r="J15" s="151">
         <v>732</v>
       </c>
-      <c r="K15" s="156" t="s">
-        <v>865</v>
+      <c r="K15" s="161" t="s">
+        <v>881</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
@@ -9875,7 +9880,7 @@
         <v>97</v>
       </c>
       <c r="G16" s="155" t="s">
-        <v>881</v>
+        <v>868</v>
       </c>
       <c r="H16" s="151" t="s">
         <v>131</v>
@@ -9886,8 +9891,8 @@
       <c r="J16" s="151">
         <v>642</v>
       </c>
-      <c r="K16" s="156" t="s">
-        <v>854</v>
+      <c r="K16" s="161" t="s">
+        <v>886</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
@@ -9910,7 +9915,7 @@
         <v>97</v>
       </c>
       <c r="G17" s="155" t="s">
-        <v>882</v>
+        <v>869</v>
       </c>
       <c r="H17" s="151" t="s">
         <v>132</v>
@@ -9921,8 +9926,8 @@
       <c r="J17" s="151">
         <v>711</v>
       </c>
-      <c r="K17" s="156" t="s">
-        <v>866</v>
+      <c r="K17" s="161" t="s">
+        <v>853</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
@@ -9945,7 +9950,7 @@
         <v>97</v>
       </c>
       <c r="G18" s="155" t="s">
-        <v>882</v>
+        <v>869</v>
       </c>
       <c r="H18" s="151" t="s">
         <v>132</v>
@@ -9956,8 +9961,8 @@
       <c r="J18" s="151">
         <v>548</v>
       </c>
-      <c r="K18" s="156" t="s">
-        <v>867</v>
+      <c r="K18" s="161" t="s">
+        <v>887</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
@@ -9980,7 +9985,7 @@
         <v>97</v>
       </c>
       <c r="G19" s="155" t="s">
-        <v>882</v>
+        <v>869</v>
       </c>
       <c r="H19" s="151" t="s">
         <v>132</v>
@@ -9991,8 +9996,8 @@
       <c r="J19" s="151">
         <v>841</v>
       </c>
-      <c r="K19" s="156" t="s">
-        <v>868</v>
+      <c r="K19" s="161" t="s">
+        <v>883</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
@@ -10015,7 +10020,7 @@
         <v>97</v>
       </c>
       <c r="G20" s="155" t="s">
-        <v>882</v>
+        <v>869</v>
       </c>
       <c r="H20" s="151" t="s">
         <v>132</v>
@@ -10026,8 +10031,8 @@
       <c r="J20" s="151">
         <v>547</v>
       </c>
-      <c r="K20" s="156" t="s">
-        <v>855</v>
+      <c r="K20" s="161" t="s">
+        <v>884</v>
       </c>
     </row>
   </sheetData>
@@ -10041,8 +10046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8F71540-D5E4-44EA-999A-40575FE3AC31}">
   <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -10919,281 +10924,281 @@
         <v>32</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>874</v>
-      </c>
-      <c r="C1" s="158" t="s">
+        <v>861</v>
+      </c>
+      <c r="C1" s="157" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="159" t="s">
-        <v>873</v>
-      </c>
-      <c r="E1" s="157"/>
-      <c r="F1" s="157"/>
-      <c r="G1" s="157"/>
+      <c r="D1" s="158" t="s">
+        <v>860</v>
+      </c>
+      <c r="E1" s="156"/>
+      <c r="F1" s="156"/>
+      <c r="G1" s="156"/>
     </row>
     <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A2" s="160" t="s">
+      <c r="A2" s="159" t="s">
         <v>99</v>
       </c>
-      <c r="B2" s="160" t="s">
+      <c r="B2" s="159" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="161" t="s">
-        <v>875</v>
-      </c>
-      <c r="D2" s="160" t="s">
+      <c r="C2" s="160" t="s">
+        <v>862</v>
+      </c>
+      <c r="D2" s="159" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A3" s="160" t="s">
+      <c r="A3" s="159" t="s">
         <v>100</v>
       </c>
-      <c r="B3" s="160" t="s">
+      <c r="B3" s="159" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="161" t="s">
-        <v>875</v>
-      </c>
-      <c r="D3" s="160" t="s">
+      <c r="C3" s="160" t="s">
+        <v>862</v>
+      </c>
+      <c r="D3" s="159" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A4" s="160" t="s">
+      <c r="A4" s="159" t="s">
         <v>101</v>
       </c>
-      <c r="B4" s="160" t="s">
+      <c r="B4" s="159" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="161" t="s">
-        <v>875</v>
-      </c>
-      <c r="D4" s="160" t="s">
+      <c r="C4" s="160" t="s">
+        <v>862</v>
+      </c>
+      <c r="D4" s="159" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A5" s="160" t="s">
+      <c r="A5" s="159" t="s">
         <v>102</v>
       </c>
-      <c r="B5" s="160" t="s">
+      <c r="B5" s="159" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="161" t="s">
-        <v>877</v>
-      </c>
-      <c r="D5" s="160" t="s">
+      <c r="C5" s="160" t="s">
+        <v>864</v>
+      </c>
+      <c r="D5" s="159" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A6" s="160" t="s">
+      <c r="A6" s="159" t="s">
         <v>103</v>
       </c>
-      <c r="B6" s="160" t="s">
+      <c r="B6" s="159" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="161" t="s">
-        <v>877</v>
-      </c>
-      <c r="D6" s="160" t="s">
+      <c r="C6" s="160" t="s">
+        <v>864</v>
+      </c>
+      <c r="D6" s="159" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A7" s="160" t="s">
+      <c r="A7" s="159" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="160" t="s">
+      <c r="B7" s="159" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="161" t="s">
-        <v>877</v>
-      </c>
-      <c r="D7" s="160" t="s">
+      <c r="C7" s="160" t="s">
+        <v>864</v>
+      </c>
+      <c r="D7" s="159" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A8" s="160" t="s">
+      <c r="A8" s="159" t="s">
         <v>105</v>
       </c>
-      <c r="B8" s="160" t="s">
+      <c r="B8" s="159" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="161" t="s">
-        <v>875</v>
-      </c>
-      <c r="D8" s="160" t="s">
+      <c r="C8" s="160" t="s">
+        <v>862</v>
+      </c>
+      <c r="D8" s="159" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A9" s="160" t="s">
+      <c r="A9" s="159" t="s">
         <v>106</v>
       </c>
-      <c r="B9" s="160" t="s">
+      <c r="B9" s="159" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="161" t="s">
-        <v>875</v>
-      </c>
-      <c r="D9" s="160" t="s">
+      <c r="C9" s="160" t="s">
+        <v>862</v>
+      </c>
+      <c r="D9" s="159" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A10" s="160" t="s">
+      <c r="A10" s="159" t="s">
         <v>107</v>
       </c>
-      <c r="B10" s="160" t="s">
+      <c r="B10" s="159" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="161" t="s">
-        <v>875</v>
-      </c>
-      <c r="D10" s="160" t="s">
+      <c r="C10" s="160" t="s">
+        <v>862</v>
+      </c>
+      <c r="D10" s="159" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A11" s="160" t="s">
+      <c r="A11" s="159" t="s">
         <v>108</v>
       </c>
-      <c r="B11" s="160" t="s">
+      <c r="B11" s="159" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="161" t="s">
-        <v>877</v>
-      </c>
-      <c r="D11" s="160" t="s">
+      <c r="C11" s="160" t="s">
+        <v>864</v>
+      </c>
+      <c r="D11" s="159" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A12" s="160" t="s">
+      <c r="A12" s="159" t="s">
         <v>109</v>
       </c>
-      <c r="B12" s="160" t="s">
+      <c r="B12" s="159" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="161" t="s">
-        <v>877</v>
-      </c>
-      <c r="D12" s="160" t="s">
+      <c r="C12" s="160" t="s">
+        <v>864</v>
+      </c>
+      <c r="D12" s="159" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A13" s="160" t="s">
+      <c r="A13" s="159" t="s">
         <v>110</v>
       </c>
-      <c r="B13" s="160" t="s">
+      <c r="B13" s="159" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="161" t="s">
-        <v>877</v>
-      </c>
-      <c r="D13" s="160" t="s">
+      <c r="C13" s="160" t="s">
+        <v>864</v>
+      </c>
+      <c r="D13" s="159" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A14" s="160" t="s">
+      <c r="A14" s="159" t="s">
         <v>111</v>
       </c>
-      <c r="B14" s="160" t="s">
+      <c r="B14" s="159" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="161" t="s">
-        <v>877</v>
-      </c>
-      <c r="D14" s="160" t="s">
+      <c r="C14" s="160" t="s">
+        <v>864</v>
+      </c>
+      <c r="D14" s="159" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A15" s="160" t="s">
+      <c r="A15" s="159" t="s">
         <v>112</v>
       </c>
-      <c r="B15" s="160" t="s">
+      <c r="B15" s="159" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="161" t="s">
-        <v>876</v>
-      </c>
-      <c r="D15" s="160" t="s">
+      <c r="C15" s="160" t="s">
+        <v>863</v>
+      </c>
+      <c r="D15" s="159" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A16" s="160" t="s">
+      <c r="A16" s="159" t="s">
         <v>113</v>
       </c>
-      <c r="B16" s="160" t="s">
+      <c r="B16" s="159" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="161" t="s">
-        <v>876</v>
-      </c>
-      <c r="D16" s="160" t="s">
+      <c r="C16" s="160" t="s">
+        <v>863</v>
+      </c>
+      <c r="D16" s="159" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A17" s="160" t="s">
+      <c r="A17" s="159" t="s">
         <v>114</v>
       </c>
-      <c r="B17" s="160" t="s">
+      <c r="B17" s="159" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="161" t="s">
-        <v>876</v>
-      </c>
-      <c r="D17" s="160" t="s">
+      <c r="C17" s="160" t="s">
+        <v>863</v>
+      </c>
+      <c r="D17" s="159" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A18" s="160" t="s">
+      <c r="A18" s="159" t="s">
         <v>115</v>
       </c>
-      <c r="B18" s="160" t="s">
+      <c r="B18" s="159" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="161" t="s">
-        <v>876</v>
-      </c>
-      <c r="D18" s="160" t="s">
+      <c r="C18" s="160" t="s">
+        <v>863</v>
+      </c>
+      <c r="D18" s="159" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A19" s="160" t="s">
+      <c r="A19" s="159" t="s">
         <v>116</v>
       </c>
-      <c r="B19" s="160" t="s">
+      <c r="B19" s="159" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="161" t="s">
-        <v>876</v>
-      </c>
-      <c r="D19" s="160" t="s">
+      <c r="C19" s="160" t="s">
+        <v>863</v>
+      </c>
+      <c r="D19" s="159" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A20" s="160" t="s">
+      <c r="A20" s="159" t="s">
         <v>117</v>
       </c>
-      <c r="B20" s="160" t="s">
+      <c r="B20" s="159" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="161" t="s">
-        <v>876</v>
-      </c>
-      <c r="D20" s="160" t="s">
+      <c r="C20" s="160" t="s">
+        <v>863</v>
+      </c>
+      <c r="D20" s="159" t="s">
         <v>41</v>
       </c>
     </row>
@@ -27465,7 +27470,7 @@
         <v>118</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>869</v>
+        <v>856</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>